<commit_message>
Belfort_v2 including European buildings
</commit_message>
<xml_diff>
--- a/Models/Belfort_v2/Conso/Bati/Europe/Parameters_residential.xlsx
+++ b/Models/Belfort_v2/Conso/Bati/Europe/Parameters_residential.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickdartois/Documents/Corps des Mines/3A/Mémoire 3A/Modèle/Energy-Alternatives-Planing/Models/Belfort_v2/Conso/Bati/Europe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7723390-9431-D44B-8DFE-8F2ACD53A4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF54AE63-4204-4449-A566-80C12FCDE862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="23880" windowHeight="14080" activeTab="1" xr2:uid="{B94D5A13-5B0A-0448-8917-C62227F4AC01}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="23880" windowHeight="14080" firstSheet="1" activeTab="9" xr2:uid="{B94D5A13-5B0A-0448-8917-C62227F4AC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Number_of_households" sheetId="1" r:id="rId1"/>
     <sheet name="Energy_per_sqm" sheetId="2" r:id="rId2"/>
     <sheet name="Factors" sheetId="3" r:id="rId3"/>
-    <sheet name="RES_hh_num" sheetId="4" r:id="rId4"/>
-    <sheet name="Heating_degree_days" sheetId="7" r:id="rId5"/>
-    <sheet name="RES_hh_fecs" sheetId="6" r:id="rId6"/>
-    <sheet name="Indicators" sheetId="8" r:id="rId7"/>
-    <sheet name="RES_hh_tes" sheetId="5" r:id="rId8"/>
+    <sheet name="Threshold_renovation" sheetId="9" r:id="rId4"/>
+    <sheet name="RES_hh_num" sheetId="4" r:id="rId5"/>
+    <sheet name="Heating_degree_days" sheetId="7" r:id="rId6"/>
+    <sheet name="RES_hh_fecs" sheetId="6" r:id="rId7"/>
+    <sheet name="Indicators" sheetId="8" r:id="rId8"/>
+    <sheet name="RES_hh_tes" sheetId="5" r:id="rId9"/>
+    <sheet name="Efficiency" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="62">
   <si>
     <t>AREA</t>
   </si>
@@ -175,12 +177,66 @@
   <si>
     <t>COP</t>
   </si>
+  <si>
+    <t>Heating_degree_days</t>
+  </si>
+  <si>
+    <t>French Data</t>
+  </si>
+  <si>
+    <t>Heating degree days (2000-2015)</t>
+  </si>
+  <si>
+    <t>Threshold class C-D (kWh/m2)</t>
+  </si>
+  <si>
+    <t>Consumption reduction factor (class C)</t>
+  </si>
+  <si>
+    <t>Consumption reduction factor (class D)</t>
+  </si>
+  <si>
+    <t>Part of heating in energy consumption</t>
+  </si>
+  <si>
+    <t>Threshold (kWh/m2)</t>
+  </si>
+  <si>
+    <t>Threshold (kWh/m2/heating degree-days)</t>
+  </si>
+  <si>
+    <t>Threshold_renovation</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Efficiency progress 2010-2015</t>
+  </si>
+  <si>
+    <t>Number of households</t>
+  </si>
+  <si>
+    <t>Number of renovations/year</t>
+  </si>
+  <si>
+    <t>Energy efficiency gain per renovation 2012-2016</t>
+  </si>
+  <si>
+    <t>Renovation rate 2012-2016</t>
+  </si>
+  <si>
+    <t>Global efficiency gain 2012-2016</t>
+  </si>
+  <si>
+    <t>Number of complete renovations/year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +249,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="161"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,16 +275,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B2A58E6A-7648-9441-B2BE-EAE56FD94E50}"/>
+    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,7 +606,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,6 +1333,564 @@
       <c r="D46">
         <f>SUMIFS(Indicators!R:R,Indicators!B:B,"Households useful surface area (in sqm/household)",Indicators!A:A,Number_of_households!A46)</f>
         <v>94.439881098473975</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927C7A5D-4F18-2C4E-B9A3-96E44134D907}">
+  <dimension ref="A1:Y7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>2000</v>
+      </c>
+      <c r="C1">
+        <v>2001</v>
+      </c>
+      <c r="D1">
+        <v>2002</v>
+      </c>
+      <c r="E1">
+        <v>2003</v>
+      </c>
+      <c r="F1">
+        <v>2004</v>
+      </c>
+      <c r="G1">
+        <v>2005</v>
+      </c>
+      <c r="H1">
+        <v>2006</v>
+      </c>
+      <c r="I1">
+        <v>2007</v>
+      </c>
+      <c r="J1">
+        <v>2008</v>
+      </c>
+      <c r="K1">
+        <v>2009</v>
+      </c>
+      <c r="L1">
+        <v>2010</v>
+      </c>
+      <c r="M1">
+        <v>2011</v>
+      </c>
+      <c r="N1">
+        <v>2012</v>
+      </c>
+      <c r="O1">
+        <v>2013</v>
+      </c>
+      <c r="P1">
+        <v>2014</v>
+      </c>
+      <c r="Q1">
+        <v>2015</v>
+      </c>
+      <c r="R1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0.6079014827324305</v>
+      </c>
+      <c r="C2">
+        <v>0.61324853118128919</v>
+      </c>
+      <c r="D2">
+        <v>0.62536682278641575</v>
+      </c>
+      <c r="E2">
+        <v>0.62814261759250245</v>
+      </c>
+      <c r="F2">
+        <v>0.63449560765924928</v>
+      </c>
+      <c r="G2">
+        <v>0.6393721757462979</v>
+      </c>
+      <c r="H2">
+        <v>0.63994711440845964</v>
+      </c>
+      <c r="I2">
+        <v>0.64384023862584538</v>
+      </c>
+      <c r="J2">
+        <v>0.64121977400629715</v>
+      </c>
+      <c r="K2">
+        <v>0.64924672841758646</v>
+      </c>
+      <c r="L2">
+        <v>0.65476049789315904</v>
+      </c>
+      <c r="M2">
+        <v>0.66111168635483641</v>
+      </c>
+      <c r="N2">
+        <v>0.67010148014597415</v>
+      </c>
+      <c r="O2">
+        <v>0.67858200810425351</v>
+      </c>
+      <c r="P2">
+        <v>0.69309902925963507</v>
+      </c>
+      <c r="Q2">
+        <v>0.70484385024488727</v>
+      </c>
+      <c r="R2">
+        <f>(Q2-L2)/5</f>
+        <v>1.0016670470345646E-2</v>
+      </c>
+      <c r="S2">
+        <f>SUMIFS(Number_of_households!C:C,Number_of_households!A:A,Efficiency!A2)</f>
+        <v>4920537.9999999944</v>
+      </c>
+      <c r="T2">
+        <f>R2/R$7*S2/S$7*T$7</f>
+        <v>72931.27599276838</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="W2" s="5">
+        <v>0.156</v>
+      </c>
+      <c r="X2" s="5">
+        <f>V2*W2</f>
+        <v>1.4039999999999999E-2</v>
+      </c>
+      <c r="Y2">
+        <f>ROUND(X2/X$7*S2/S$7*Y$7,0)</f>
+        <v>84814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>0.70403602951657684</v>
+      </c>
+      <c r="C3">
+        <v>0.70485540481423159</v>
+      </c>
+      <c r="D3">
+        <v>0.70900156027557337</v>
+      </c>
+      <c r="E3">
+        <v>0.70810036266493503</v>
+      </c>
+      <c r="F3">
+        <v>0.7147567779404983</v>
+      </c>
+      <c r="G3">
+        <v>0.71685455392703756</v>
+      </c>
+      <c r="H3">
+        <v>0.71613913145143882</v>
+      </c>
+      <c r="I3">
+        <v>0.72501330076164527</v>
+      </c>
+      <c r="J3">
+        <v>0.72287444231095321</v>
+      </c>
+      <c r="K3">
+        <v>0.72702304796264783</v>
+      </c>
+      <c r="L3">
+        <v>0.73146015662418995</v>
+      </c>
+      <c r="M3">
+        <v>0.73707886876215412</v>
+      </c>
+      <c r="N3">
+        <v>0.7410928299778865</v>
+      </c>
+      <c r="O3">
+        <v>0.74997442107786028</v>
+      </c>
+      <c r="P3">
+        <v>0.75491235192121442</v>
+      </c>
+      <c r="Q3">
+        <v>0.76225185997982992</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R7" si="0">(Q3-L3)/5</f>
+        <v>6.1583406711279935E-3</v>
+      </c>
+      <c r="S3">
+        <f>SUMIFS(Number_of_households!C:C,Number_of_households!A:A,Efficiency!A3)</f>
+        <v>40558210</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T6" si="1">R3/R$7*S3/S$7*T$7</f>
+        <v>369590.09591920831</v>
+      </c>
+      <c r="V3" s="5">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="W3" s="5">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="X3" s="5">
+        <f t="shared" ref="X3:X7" si="2">V3*W3</f>
+        <v>8.7220000000000006E-3</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y6" si="3">ROUND(X3/X$7*S3/S$7*Y$7,0)</f>
+        <v>434293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0.54039159523757196</v>
+      </c>
+      <c r="C4">
+        <v>0.55581250162517892</v>
+      </c>
+      <c r="D4">
+        <v>0.55951464564221265</v>
+      </c>
+      <c r="E4">
+        <v>0.56825786251451416</v>
+      </c>
+      <c r="F4">
+        <v>0.57544189067188178</v>
+      </c>
+      <c r="G4">
+        <v>0.58638566372550316</v>
+      </c>
+      <c r="H4">
+        <v>0.603296452613034</v>
+      </c>
+      <c r="I4">
+        <v>0.60967622099484775</v>
+      </c>
+      <c r="J4">
+        <v>0.61442261690603706</v>
+      </c>
+      <c r="K4">
+        <v>0.61363853804812885</v>
+      </c>
+      <c r="L4">
+        <v>0.63348618370444676</v>
+      </c>
+      <c r="M4">
+        <v>0.6417322077740425</v>
+      </c>
+      <c r="N4">
+        <v>0.64730384036343458</v>
+      </c>
+      <c r="O4">
+        <v>0.6484200092272816</v>
+      </c>
+      <c r="P4">
+        <v>0.66062258791290285</v>
+      </c>
+      <c r="Q4">
+        <v>0.66665213904684761</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>6.6331910684801713E-3</v>
+      </c>
+      <c r="S4">
+        <f>SUMIFS(Number_of_households!C:C,Number_of_households!A:A,Efficiency!A4)</f>
+        <v>18579825.999999993</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>182365.20750335132</v>
+      </c>
+      <c r="V4" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="X4" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1900000000000003E-2</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="3"/>
+        <v>271442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0.63425224953512604</v>
+      </c>
+      <c r="C5">
+        <v>0.63954695124403793</v>
+      </c>
+      <c r="D5">
+        <v>0.64367619840305046</v>
+      </c>
+      <c r="E5">
+        <v>0.65326815196831645</v>
+      </c>
+      <c r="F5">
+        <v>0.65809031805246754</v>
+      </c>
+      <c r="G5">
+        <v>0.66560725160305689</v>
+      </c>
+      <c r="H5">
+        <v>0.67028200473938193</v>
+      </c>
+      <c r="I5">
+        <v>0.6753714071351099</v>
+      </c>
+      <c r="J5">
+        <v>0.67692294478690751</v>
+      </c>
+      <c r="K5">
+        <v>0.68309288229845977</v>
+      </c>
+      <c r="L5">
+        <v>0.68666768005096457</v>
+      </c>
+      <c r="M5">
+        <v>0.69422352396260456</v>
+      </c>
+      <c r="N5">
+        <v>0.7003388006163086</v>
+      </c>
+      <c r="O5">
+        <v>0.70582151781336167</v>
+      </c>
+      <c r="P5">
+        <v>0.71525338614900957</v>
+      </c>
+      <c r="Q5">
+        <v>0.72396704506346821</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>7.4598730025007276E-3</v>
+      </c>
+      <c r="S5">
+        <f>SUMIFS(Number_of_households!C:C,Number_of_households!A:A,Efficiency!A5)</f>
+        <v>27891301.000000015</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>307877.56422077236</v>
+      </c>
+      <c r="V5" s="5">
+        <v>0.114</v>
+      </c>
+      <c r="W5" s="5">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="X5" s="5">
+        <f t="shared" si="2"/>
+        <v>9.0060000000000001E-3</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="3"/>
+        <v>308382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0.59143749869227558</v>
+      </c>
+      <c r="C6">
+        <v>0.5952968761420947</v>
+      </c>
+      <c r="D6">
+        <v>0.59585259054436468</v>
+      </c>
+      <c r="E6">
+        <v>0.59922060714078862</v>
+      </c>
+      <c r="F6">
+        <v>0.6129262540819459</v>
+      </c>
+      <c r="G6">
+        <v>0.6107698650484521</v>
+      </c>
+      <c r="H6">
+        <v>0.60985523806214081</v>
+      </c>
+      <c r="I6">
+        <v>0.60509902144398287</v>
+      </c>
+      <c r="J6">
+        <v>0.60658450721357038</v>
+      </c>
+      <c r="K6">
+        <v>0.61421011799523384</v>
+      </c>
+      <c r="L6">
+        <v>0.62499833162575258</v>
+      </c>
+      <c r="M6">
+        <v>0.64446544642521086</v>
+      </c>
+      <c r="N6">
+        <v>0.6414538995997412</v>
+      </c>
+      <c r="O6">
+        <v>0.64920275234609814</v>
+      </c>
+      <c r="P6">
+        <v>0.65350464703376876</v>
+      </c>
+      <c r="Q6">
+        <v>0.66115687088235686</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>7.2317078513208562E-3</v>
+      </c>
+      <c r="S6">
+        <f>SUMIFS(Number_of_households!C:C,Number_of_households!A:A,Efficiency!A6)</f>
+        <v>25782702.000000004</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>275897.10117274051</v>
+      </c>
+      <c r="V6" s="5">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="X6" s="5">
+        <f t="shared" si="2"/>
+        <v>1.3426000000000002E-2</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="3"/>
+        <v>424975</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>0.62494385183155843</v>
+      </c>
+      <c r="C7">
+        <v>0.63100488223944085</v>
+      </c>
+      <c r="D7">
+        <v>0.63903273752505019</v>
+      </c>
+      <c r="E7">
+        <v>0.64348538190652738</v>
+      </c>
+      <c r="F7">
+        <v>0.64952006483220326</v>
+      </c>
+      <c r="G7">
+        <v>0.65193683298608884</v>
+      </c>
+      <c r="H7">
+        <v>0.66021240588512276</v>
+      </c>
+      <c r="I7">
+        <v>0.66509731887154944</v>
+      </c>
+      <c r="J7">
+        <v>0.67260653041873542</v>
+      </c>
+      <c r="K7">
+        <v>0.67502227850841845</v>
+      </c>
+      <c r="L7">
+        <v>0.68498274259380232</v>
+      </c>
+      <c r="M7">
+        <v>0.68775361267503599</v>
+      </c>
+      <c r="N7">
+        <v>0.69987408452036171</v>
+      </c>
+      <c r="O7">
+        <v>0.71108618752861052</v>
+      </c>
+      <c r="P7">
+        <v>0.71535580582122094</v>
+      </c>
+      <c r="Q7">
+        <v>0.72967345395685357</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>8.93814227261025E-3</v>
+      </c>
+      <c r="S7" s="4">
+        <v>30243698</v>
+      </c>
+      <c r="T7">
+        <f>400000</f>
+        <v>400000</v>
+      </c>
+      <c r="V7" s="5">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="X7" s="5">
+        <f t="shared" si="2"/>
+        <v>1.0773000000000001E-2</v>
+      </c>
+      <c r="Y7">
+        <v>400000</v>
       </c>
     </row>
   </sheetData>
@@ -1274,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ECB79D-7FBE-364B-81F8-62BECD0F82B6}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1828,13 +2456,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A6457F-535E-1F4E-9DD5-D15BBDC8DC3D}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1844,8 +2474,14 @@
       <c r="C1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1856,8 +2492,16 @@
       <c r="C2">
         <v>2.6619999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>AVERAGE(Heating_degree_days!C2:R2)</f>
+        <v>2663.3512500000002</v>
+      </c>
+      <c r="E2">
+        <f>D2*Threshold_renovation!$B$8</f>
+        <v>108.79752716405025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1868,8 +2512,16 @@
       <c r="C3">
         <v>2.653</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f>AVERAGE(Heating_degree_days!C5:R5)</f>
+        <v>3048.9612499999998</v>
+      </c>
+      <c r="E3">
+        <f>D3*Threshold_renovation!$B$8</f>
+        <v>124.54964189158736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1880,8 +2532,16 @@
       <c r="C4">
         <v>2.0129999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f>AVERAGE(Heating_degree_days!C8:R8)</f>
+        <v>1794.6593750000002</v>
+      </c>
+      <c r="E4">
+        <f>D4*Threshold_renovation!$B$8</f>
+        <v>73.311585207463693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1892,8 +2552,16 @@
       <c r="C5">
         <v>2.581</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>AVERAGE(Heating_degree_days!C14:R14)</f>
+        <v>2998.5081250000003</v>
+      </c>
+      <c r="E5">
+        <f>D5*Threshold_renovation!$B$8</f>
+        <v>122.48863877091424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1903,6 +2571,14 @@
       </c>
       <c r="C6">
         <v>2.2930000000000001</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE(Heating_degree_days!C11:R11)</f>
+        <v>1914.2137499999999</v>
+      </c>
+      <c r="E6">
+        <f>D6*Threshold_renovation!$B$8</f>
+        <v>78.19536475462013</v>
       </c>
     </row>
   </sheetData>
@@ -1911,11 +2587,90 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92589632-3CB6-114D-AB8A-69D7603A38CA}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>2371.183125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2">
+        <f>1-0.1356-0.0034</f>
+        <v>0.8610000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <f>B3*B4*(1-B6)</f>
+        <v>96.862500000000011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <f>B7/B2</f>
+        <v>4.0849860552208517E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BFED56-CD45-B044-90DE-6DD48E9725AF}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4779,12 +5534,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEEE157-521F-8F4A-BF71-22A465181D06}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5283,7 +6038,7 @@
       <c r="Q9">
         <v>1847.4219444444445</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="3">
         <v>1847.4219444444445</v>
       </c>
     </row>
@@ -5684,11 +6439,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC010DCC-FE71-3F45-B785-8E7990F771F6}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
@@ -8829,7 +9584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5857AAEC-7785-6D45-860D-38A4CFF43A61}">
   <dimension ref="A1:R41"/>
   <sheetViews>
@@ -11134,13 +11889,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B369D7A-042D-0849-8133-437371CC6B75}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>